<commit_message>
updating this old repo
</commit_message>
<xml_diff>
--- a/ENTORNO DE OPCIONES/data/boards/gtamani_board.xlsx
+++ b/ENTORNO DE OPCIONES/data/boards/gtamani_board.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:F1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,30 +434,93 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Opcion</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Opcion</t>
+          <t>Side</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Side</t>
+          <t>Strike</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Base</t>
+          <t>Price</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Precio</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Strike</t>
-        </is>
+          <t>Cant</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>GFGC100OCT</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>GFGC120OCT</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>120</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>GFGV80OCT</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>80</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>